<commit_message>
Implement j/k scrolling features
</commit_message>
<xml_diff>
--- a/AHK scripts (version 1).xlsx
+++ b/AHK scripts (version 1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuanc\Desktop\In current use\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuanc\Desktop\Coding folder\In current use\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0159A2-1F9E-4BB3-A81E-3AB6004B7DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD6639A-63A7-418D-9F5D-BA1C79DA666D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" activeTab="4" xr2:uid="{930CD8CA-213E-40C1-995B-A96F7B5469F9}"/>
+    <workbookView xWindow="2263" yWindow="2263" windowWidth="24686" windowHeight="14597" activeTab="4" xr2:uid="{930CD8CA-213E-40C1-995B-A96F7B5469F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hotkeys" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,18 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={FFD3FD5D-4306-4F55-BBFC-605379500C34}</author>
+    <author>tc={D36A1414-AE86-4CF5-B8AA-C18879408D12}</author>
   </authors>
   <commentList>
     <comment ref="D3" authorId="0" shapeId="0" xr:uid="{FFD3FD5D-4306-4F55-BBFC-605379500C34}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Distance + whether I can use with one hand</t>
+      </text>
+    </comment>
+    <comment ref="D53" authorId="1" shapeId="0" xr:uid="{D36A1414-AE86-4CF5-B8AA-C18879408D12}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -59,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="463">
   <si>
     <t>Hotkey</t>
   </si>
@@ -1449,6 +1458,9 @@
   </si>
   <si>
     <t>timestamps inc vid</t>
+  </si>
+  <si>
+    <t>[key held down]</t>
   </si>
 </sst>
 </file>
@@ -2004,6 +2016,9 @@
   <threadedComment ref="D3" dT="2022-06-20T15:57:20.78" personId="{6AAC6723-9AE5-4045-B618-C6F9115F84E3}" id="{FFD3FD5D-4306-4F55-BBFC-605379500C34}">
     <text>Distance + whether I can use with one hand</text>
   </threadedComment>
+  <threadedComment ref="D53" dT="2022-06-20T15:57:20.78" personId="{6AAC6723-9AE5-4045-B618-C6F9115F84E3}" id="{D36A1414-AE86-4CF5-B8AA-C18879408D12}">
+    <text>Distance + whether I can use with one hand</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -4512,10 +4527,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479BA172-A34C-4863-AE01-6F1CE078F84E}">
-  <dimension ref="A3:L41"/>
+  <dimension ref="A3:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5089,6 +5104,207 @@
         <v>458</v>
       </c>
     </row>
+    <row r="53" spans="1:5" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A53" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A54" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A55" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A56" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A57" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A58" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A59" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A60" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A61" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A62" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A63" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A64" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A65" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A66" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A67" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A68" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A69" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A70" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A71" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A72" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A73" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A74" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A75" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A76" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A77" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A78" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A79" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A81" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A82" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A83" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A84" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A85" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A86" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A87" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A88" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A89" s="1">
+        <v>0</v>
+      </c>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>